<commit_message>
masukin data2 dari dokumen bapak beres update database/sipepeng_full_isi_25-5-2015.sql
</commit_message>
<xml_diff>
--- a/DOKUMEN  PENDUKUNG/DATA DATA YANG HARUS DIMASUKAN/DATA LAPANGAN/DATA validasi USULAN PEMBANGUNAN_perencaan.xlsx
+++ b/DOKUMEN  PENDUKUNG/DATA DATA YANG HARUS DIMASUKAN/DATA LAPANGAN/DATA validasi USULAN PEMBANGUNAN_perencaan.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\sipepeng\DOKUMEN  PENDUKUNG\DATA DATA YANG HARUS DIMASUKAN\DATA LAPANGAN\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010" tabRatio="762" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010" tabRatio="762" firstSheet="6" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="JALAN 2015" sheetId="1" r:id="rId1"/>
@@ -1528,6 +1533,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -1575,7 +1583,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1610,7 +1618,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -4437,7 +4445,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M10"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="80" zoomScaleSheetLayoutView="80" workbookViewId="0">
+    <sheetView view="pageBreakPreview" zoomScale="80" zoomScaleSheetLayoutView="80" workbookViewId="0">
       <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
@@ -4730,8 +4738,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L10"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScale="80" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView view="pageBreakPreview" topLeftCell="E1" zoomScale="80" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5393,7 +5401,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L13"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScale="80" zoomScaleSheetLayoutView="80" workbookViewId="0">
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="80" zoomScaleSheetLayoutView="80" workbookViewId="0">
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>

</xml_diff>